<commit_message>
organizing project into three layers (command , Logic , revit)
</commit_message>
<xml_diff>
--- a/RevitProject/first excel.xlsx
+++ b/RevitProject/first excel.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Bim2\RevitAPI\SelfStudy\RevitApp\RevitApi-CreateSheets-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Bim2\RevitAPI\labs and lectures\RevitApiProject\RevitProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CDB8B1-E816-4A8B-9C2A-4F6011401038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5976F123-958E-4536-A342-F1206196B928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="second sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="revitSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EED45FA3-15F1-44F1-90E4-B2D3424D8106}" name="RevitData" displayName="RevitData" ref="D6:F14" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EED45FA3-15F1-44F1-90E4-B2D3424D8106}" name="revitData" displayName="revitData" ref="D6:F14" totalsRowShown="0">
   <autoFilter ref="D6:F14" xr:uid="{5B1A8765-C7D2-4ACA-A257-6364027D5371}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{425F391C-8F0C-4B98-B5D7-D1276EA27B6C}" name="ViewPlan"/>
@@ -470,7 +470,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>